<commit_message>
updated the descritpion and database for class and hydrology ini file creation
</commit_message>
<xml_diff>
--- a/MESHpyPreProcessing/meshparametersvalues2.xlsx
+++ b/MESHpyPreProcessing/meshparametersvalues2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YassinF\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\GitHub\Repos\MESH-Scripts-PyLib\MESHpyPreProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67ACC42-CBB4-4E19-BE0B-2592AEE76858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9464CC30-554B-46DB-AEAA-FDE1DDF58647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AC73AADA-9DAA-4E49-8D0A-BF563EF11B8B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AC73AADA-9DAA-4E49-8D0A-BF563EF11B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="class_ini" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="138">
   <si>
     <t>fcan</t>
   </si>
@@ -168,15 +168,6 @@
     <t>gro</t>
   </si>
   <si>
-    <t>{60,60,40}</t>
-  </si>
-  <si>
-    <t>{15,15,25}</t>
-  </si>
-  <si>
-    <t>{5,5,5}</t>
-  </si>
-  <si>
     <t>{0,0,0}</t>
   </si>
   <si>
@@ -369,7 +360,97 @@
     <t>{0,0,0,0,0}</t>
   </si>
   <si>
-    <t>channel_routing_active</t>
+    <t>{22,22,22}</t>
+  </si>
+  <si>
+    <t>{35,35,35}</t>
+  </si>
+  <si>
+    <t>{73,45,66}</t>
+  </si>
+  <si>
+    <t>{6.4,29.6,20.44}</t>
+  </si>
+  <si>
+    <t>{7.4,0,0}</t>
+  </si>
+  <si>
+    <t>{4,2,1}</t>
+  </si>
+  <si>
+    <t>{-4,-4,-4}</t>
+  </si>
+  <si>
+    <t>{16,20,20}</t>
+  </si>
+  <si>
+    <t>{-4,-6,-8}</t>
+  </si>
+  <si>
+    <t>{50,50,40}</t>
+  </si>
+  <si>
+    <t>{15,25,25}</t>
+  </si>
+  <si>
+    <t>{5,20,30}</t>
+  </si>
+  <si>
+    <t>{30,30,30}</t>
+  </si>
+  <si>
+    <t>{60,60,60}</t>
+  </si>
+  <si>
+    <t>LichenMossG</t>
+  </si>
+  <si>
+    <t>{72.1,49.7,70.02}</t>
+  </si>
+  <si>
+    <t>{5.0,21.4,23.682}</t>
+  </si>
+  <si>
+    <t>{7.8,0,0}</t>
+  </si>
+  <si>
+    <t>{50,55,60}</t>
+  </si>
+  <si>
+    <t>{15,10,5}</t>
+  </si>
+  <si>
+    <t>{73.2,43.3,72.903}</t>
+  </si>
+  <si>
+    <t>{5.2,29.10,21.362}</t>
+  </si>
+  <si>
+    <t>{5,0,0}</t>
+  </si>
+  <si>
+    <t>{75,66,66}</t>
+  </si>
+  <si>
+    <t>{5,30,17}</t>
+  </si>
+  <si>
+    <t>{0.1,0.045,0.049,0.013,0.05,0.15,0.141,0.150,0.135,0.314}</t>
+  </si>
+  <si>
+    <t>{0.2,0.167,0.156,0.049,0.064,0.596,0.514,0.422,0.171,0.544}</t>
+  </si>
+  <si>
+    <t>{0.000079,0.000076,0.000016,0.000018,0.00006,.0000042,0.000042,0.000042,0.000042,0.000042}</t>
+  </si>
+  <si>
+    <t>{1.618,2.570,2.721,2.993,2.823,1.361,1.361,1.361,1.361,1.361}</t>
+  </si>
+  <si>
+    <t>GRU_class_dependent_header</t>
+  </si>
+  <si>
+    <t>GRU_class_dependent_active</t>
   </si>
 </sst>
 </file>
@@ -391,12 +472,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -411,9 +498,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,24 +837,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387FA987-722D-4DBF-92F1-455064DAEB65}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -773,34 +869,37 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -835,13 +934,16 @@
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -873,46 +975,52 @@
       <c r="L3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
         <v>58</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="M4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,426 +1057,462 @@
       <c r="L5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1.1619999999999999</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>4.1479999999999997</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>4.1479999999999997</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>5.8070000000000004</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>2.3450000000000002</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7">
-        <v>0.40500000000000003</v>
+        <v>-0.187</v>
       </c>
       <c r="C7">
-        <v>0.40500000000000003</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="D7">
-        <v>0.40500000000000003</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="E7">
-        <v>0.40500000000000003</v>
+        <v>-2.5409999999999999</v>
       </c>
       <c r="F7">
-        <v>0.40500000000000003</v>
+        <v>-2.806</v>
       </c>
       <c r="G7">
-        <v>0.40500000000000003</v>
+        <v>0.3</v>
       </c>
       <c r="H7">
-        <v>0.40500000000000003</v>
+        <v>-6</v>
       </c>
       <c r="I7">
-        <v>0.40500000000000003</v>
+        <v>-5.3520000000000003</v>
       </c>
       <c r="J7">
-        <v>0.40500000000000003</v>
+        <v>-2.7309999999999999</v>
       </c>
       <c r="K7">
-        <v>0.40500000000000003</v>
+        <v>-9.1999999999999993</v>
       </c>
       <c r="L7">
-        <v>0.40500000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+      <c r="M7">
+        <v>-4.0540000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>1.6</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="C8">
-        <v>1.6</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="D8">
-        <v>1.6</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="E8">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>1.6</v>
+        <v>0.5</v>
       </c>
       <c r="G8">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>1.6</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="K8">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.03</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="C9">
-        <v>0.03</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D9">
-        <v>0.03</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E9">
-        <v>0.03</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="F9">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="G9">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="H9">
-        <v>0.03</v>
+        <v>0.2</v>
       </c>
       <c r="I9">
-        <v>0.03</v>
+        <v>0.4</v>
       </c>
       <c r="J9">
-        <v>0.03</v>
+        <v>3.1E-2</v>
       </c>
       <c r="K9">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="L9">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+      <c r="M9">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>13.624000000000001</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>23.582999999999998</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>23.582999999999998</v>
       </c>
       <c r="E10">
-        <v>12</v>
+        <v>1.923</v>
       </c>
       <c r="F10">
-        <v>12</v>
+        <v>1.2</v>
       </c>
       <c r="G10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>12</v>
+        <v>1.542</v>
       </c>
       <c r="K10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.2</v>
+      </c>
+      <c r="M10">
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.19</v>
+        <v>0.154</v>
       </c>
       <c r="C11">
-        <v>0.19</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="D11">
-        <v>0.19</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="E11">
-        <v>0.19</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="F11">
-        <v>0.19</v>
+        <v>0.34</v>
       </c>
       <c r="G11">
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="H11">
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="I11">
-        <v>0.19</v>
+        <v>0.25</v>
       </c>
       <c r="J11">
-        <v>0.19</v>
+        <v>0.255</v>
       </c>
       <c r="K11">
-        <v>0.19</v>
+        <v>0.08</v>
       </c>
       <c r="L11">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.34</v>
+      </c>
+      <c r="M11">
+        <v>0.371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.8</v>
+        <v>1.768</v>
       </c>
       <c r="C12">
-        <v>0.8</v>
+        <v>1.2490000000000001</v>
       </c>
       <c r="D12">
-        <v>0.8</v>
+        <v>1.2490000000000001</v>
       </c>
       <c r="E12">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="F12">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="G12">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>0.8</v>
+        <v>1.9410000000000001</v>
       </c>
       <c r="K12">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.2</v>
+      </c>
+      <c r="M12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B13">
-        <v>200</v>
+        <v>236.39</v>
       </c>
       <c r="C13">
-        <v>200</v>
+        <v>110.93</v>
       </c>
       <c r="D13">
-        <v>200</v>
+        <v>110.93</v>
       </c>
       <c r="E13">
-        <v>200</v>
+        <v>63.106999999999999</v>
       </c>
       <c r="F13">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G13">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>200</v>
+        <v>93.433999999999997</v>
       </c>
       <c r="K13">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="M13">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>27.913</v>
       </c>
       <c r="C14">
-        <v>30</v>
+        <v>37.506</v>
       </c>
       <c r="D14">
-        <v>30</v>
+        <v>37.506</v>
       </c>
       <c r="E14">
-        <v>30</v>
+        <v>22.541</v>
       </c>
       <c r="F14">
         <v>30</v>
       </c>
       <c r="G14">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>30</v>
+        <v>25.765000000000001</v>
       </c>
       <c r="K14">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>39.165999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.65</v>
+        <v>0.502</v>
       </c>
       <c r="C15">
-        <v>0.65</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="D15">
-        <v>0.65</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="E15">
-        <v>0.65</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="F15">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="G15">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>0.65</v>
+        <v>0.436</v>
       </c>
       <c r="K15">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="M15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B16">
-        <v>1.05</v>
+        <v>0.81200000000000006</v>
       </c>
       <c r="C16">
-        <v>1.05</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="D16">
-        <v>1.05</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="E16">
-        <v>1.05</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="F16">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>1.05</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>1.05</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>1.05</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>1.05</v>
+        <v>1.022</v>
       </c>
       <c r="K16">
-        <v>1.05</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0.749</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1388,25 +1532,28 @@
         <v>100</v>
       </c>
       <c r="G17">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>100</v>
       </c>
       <c r="K17">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1426,25 +1573,28 @@
         <v>5</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>5</v>
       </c>
       <c r="K18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1467,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1476,51 +1626,57 @@
         <v>1</v>
       </c>
       <c r="K19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B20">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="F20">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>3.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H20">
-        <v>3.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I20">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="J20">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="K20">
-        <v>3.1</v>
+        <v>10.95</v>
       </c>
       <c r="L20">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1557,8 +1713,11 @@
       <c r="L21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1572,7 +1731,7 @@
         <v>50</v>
       </c>
       <c r="E22">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F22">
         <v>50</v>
@@ -1581,7 +1740,7 @@
         <v>50</v>
       </c>
       <c r="H22">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="I22">
         <v>50</v>
@@ -1590,13 +1749,16 @@
         <v>50</v>
       </c>
       <c r="K22">
+        <v>5</v>
+      </c>
+      <c r="L22">
+        <v>5</v>
+      </c>
+      <c r="M22">
         <v>50</v>
       </c>
-      <c r="L22">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1610,145 +1772,157 @@
         <v>0.04</v>
       </c>
       <c r="E23">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="F23">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="G23">
         <v>0.04</v>
       </c>
       <c r="H23">
-        <v>0.04</v>
+        <v>1E-3</v>
       </c>
       <c r="I23">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="J23">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="K23">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="L23">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+      <c r="M23">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.71199999999999997</v>
+        <v>0.122</v>
       </c>
       <c r="C24">
-        <v>0.71199999999999997</v>
+        <v>0.1</v>
       </c>
       <c r="D24">
-        <v>0.71199999999999997</v>
+        <v>0.1</v>
       </c>
       <c r="E24">
-        <v>0.71199999999999997</v>
+        <v>0.503</v>
       </c>
       <c r="F24">
-        <v>0.71199999999999997</v>
+        <v>0.2</v>
       </c>
       <c r="G24">
-        <v>0.71199999999999997</v>
+        <v>0.1</v>
       </c>
       <c r="H24">
-        <v>0.71199999999999997</v>
+        <v>0.1</v>
       </c>
       <c r="I24">
-        <v>0.71199999999999997</v>
+        <v>0.1</v>
       </c>
       <c r="J24">
-        <v>0.71199999999999997</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="K24">
-        <v>0.71199999999999997</v>
+        <v>1</v>
       </c>
       <c r="L24">
-        <v>0.71199999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+      <c r="M24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0.29199999999999998</v>
+        <v>0.151</v>
       </c>
       <c r="C25">
-        <v>0.29199999999999998</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="D25">
-        <v>0.29199999999999998</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="E25">
-        <v>0.29199999999999998</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="F25">
-        <v>0.29199999999999998</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="G25">
-        <v>0.29199999999999998</v>
+        <v>0.01</v>
       </c>
       <c r="H25">
-        <v>0.29199999999999998</v>
+        <v>0.04</v>
       </c>
       <c r="I25">
-        <v>0.29199999999999998</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="J25">
-        <v>0.29199999999999998</v>
+        <v>0.127</v>
       </c>
       <c r="K25">
-        <v>0.29199999999999998</v>
+        <v>0.04</v>
       </c>
       <c r="L25">
-        <v>0.29199999999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.38</v>
+      </c>
+      <c r="M25">
+        <v>0.26800000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26">
-        <v>9.6000000000000002E-2</v>
+        <v>1.38</v>
       </c>
       <c r="C26">
-        <v>9.6000000000000002E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D26">
-        <v>9.6000000000000002E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E26">
-        <v>9.6000000000000002E-2</v>
+        <v>1.4319999999999999</v>
       </c>
       <c r="F26">
-        <v>9.6000000000000002E-2</v>
+        <v>0.1</v>
       </c>
       <c r="G26">
-        <v>9.6000000000000002E-2</v>
+        <v>0.01</v>
       </c>
       <c r="H26">
-        <v>9.6000000000000002E-2</v>
+        <v>0.1</v>
       </c>
       <c r="I26">
-        <v>9.6000000000000002E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J26">
-        <v>9.6000000000000002E-2</v>
+        <v>1.1639999999999999</v>
       </c>
       <c r="K26">
-        <v>9.6000000000000002E-2</v>
+        <v>1</v>
       </c>
       <c r="L26">
-        <v>9.6000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+      <c r="M26">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -1759,7 +1933,7 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -1780,355 +1954,385 @@
         <v>9</v>
       </c>
       <c r="K27">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="L27">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="F28" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="G28" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="H28" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="I28" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="J28" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="K28" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="L28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="M28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>131</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>131</v>
       </c>
       <c r="E29" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="F29" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="G29" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="H29" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="I29" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="J29" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="K29" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="L29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="M29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="E30" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="F30" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="G30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I30" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="J30" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="K30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="M30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" t="s">
+        <v>112</v>
+      </c>
+      <c r="G31" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" t="s">
+        <v>115</v>
+      </c>
+      <c r="I31" t="s">
+        <v>112</v>
+      </c>
+      <c r="J31" t="s">
+        <v>112</v>
+      </c>
+      <c r="K31" t="s">
+        <v>112</v>
+      </c>
+      <c r="L31" t="s">
+        <v>112</v>
+      </c>
+      <c r="M31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>4</v>
+      </c>
+      <c r="M32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" t="s">
-        <v>45</v>
-      </c>
-      <c r="G31" t="s">
-        <v>45</v>
-      </c>
-      <c r="H31" t="s">
-        <v>45</v>
-      </c>
-      <c r="I31" t="s">
-        <v>45</v>
-      </c>
-      <c r="J31" t="s">
-        <v>45</v>
-      </c>
-      <c r="K31" t="s">
-        <v>45</v>
-      </c>
-      <c r="L31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>4</v>
+      </c>
+      <c r="J34">
+        <v>4</v>
+      </c>
+      <c r="K34">
+        <v>4</v>
+      </c>
+      <c r="L34">
+        <v>4</v>
+      </c>
+      <c r="M34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B32">
-        <v>8</v>
-      </c>
-      <c r="C32">
-        <v>8</v>
-      </c>
-      <c r="D32">
-        <v>8</v>
-      </c>
-      <c r="E32">
-        <v>8</v>
-      </c>
-      <c r="F32">
-        <v>8</v>
-      </c>
-      <c r="G32">
-        <v>8</v>
-      </c>
-      <c r="H32">
-        <v>8</v>
-      </c>
-      <c r="I32">
-        <v>8</v>
-      </c>
-      <c r="J32">
-        <v>8</v>
-      </c>
-      <c r="K32">
-        <v>8</v>
-      </c>
-      <c r="L32">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" t="s">
+        <v>44</v>
+      </c>
+      <c r="H35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" t="s">
+        <v>44</v>
+      </c>
+      <c r="K35" t="s">
+        <v>44</v>
+      </c>
+      <c r="L35" t="s">
+        <v>44</v>
+      </c>
+      <c r="M35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B33">
-        <v>8</v>
-      </c>
-      <c r="C33">
-        <v>8</v>
-      </c>
-      <c r="D33">
-        <v>8</v>
-      </c>
-      <c r="E33">
-        <v>8</v>
-      </c>
-      <c r="F33">
-        <v>8</v>
-      </c>
-      <c r="G33">
-        <v>8</v>
-      </c>
-      <c r="H33">
-        <v>8</v>
-      </c>
-      <c r="I33">
-        <v>8</v>
-      </c>
-      <c r="J33">
-        <v>8</v>
-      </c>
-      <c r="K33">
-        <v>8</v>
-      </c>
-      <c r="L33">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34">
-        <v>8</v>
-      </c>
-      <c r="C34">
-        <v>8</v>
-      </c>
-      <c r="D34">
-        <v>8</v>
-      </c>
-      <c r="E34">
-        <v>8</v>
-      </c>
-      <c r="F34">
-        <v>8</v>
-      </c>
-      <c r="G34">
-        <v>8</v>
-      </c>
-      <c r="H34">
-        <v>8</v>
-      </c>
-      <c r="I34">
-        <v>8</v>
-      </c>
-      <c r="J34">
-        <v>8</v>
-      </c>
-      <c r="K34">
-        <v>8</v>
-      </c>
-      <c r="L34">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" t="s">
-        <v>47</v>
-      </c>
-      <c r="G35" t="s">
-        <v>47</v>
-      </c>
-      <c r="H35" t="s">
-        <v>47</v>
-      </c>
-      <c r="I35" t="s">
-        <v>47</v>
-      </c>
-      <c r="J35" t="s">
-        <v>47</v>
-      </c>
-      <c r="K35" t="s">
-        <v>47</v>
-      </c>
-      <c r="L35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="M36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -2165,8 +2369,11 @@
       <c r="L37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -2203,8 +2410,11 @@
       <c r="L38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -2241,8 +2451,11 @@
       <c r="L39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -2279,8 +2492,11 @@
       <c r="L40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -2317,8 +2533,11 @@
       <c r="L41">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -2355,8 +2574,11 @@
       <c r="L42">
         <v>100</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -2391,6 +2613,9 @@
         <v>1</v>
       </c>
       <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
         <v>1</v>
       </c>
     </row>
@@ -2405,8 +2630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363428C4-E3F0-4544-A91F-C199FAED8C49}">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,150 +2643,150 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2572,10 +2797,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2586,10 +2811,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2600,10 +2825,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2614,30 +2839,30 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
@@ -2672,48 +2897,48 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2754,142 +2979,142 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>0.1</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="E19">
-        <v>0.1</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="F19">
-        <v>0.1</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="G19">
         <v>0.1</v>
       </c>
       <c r="H19">
-        <v>0.1</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="I19">
-        <v>0.1</v>
+        <v>0.35</v>
       </c>
       <c r="J19">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="K19">
-        <v>0.1</v>
+        <v>0.218</v>
       </c>
       <c r="L19">
-        <v>0.1</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="M19">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="N19">
-        <v>0.1</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>0.1</v>
+        <v>2.3E-2</v>
       </c>
       <c r="E20">
-        <v>0.1</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="F20">
-        <v>0.1</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="G20">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="H20">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="I20">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="J20">
-        <v>0.1</v>
+        <v>3.9E-2</v>
       </c>
       <c r="K20">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="L20">
-        <v>0.1</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="M20">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="N20">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="E21">
-        <v>0.1</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="F21">
-        <v>0.1</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="G21">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H21">
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
       <c r="I21">
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
       <c r="J21">
-        <v>0.1</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="K21">
-        <v>0.1</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="L21">
-        <v>0.1</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="M21">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="N21">
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2930,10 +3155,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2974,10 +3199,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3018,10 +3243,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3062,10 +3287,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3106,10 +3331,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3150,10 +3375,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3194,10 +3419,10 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3238,10 +3463,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3282,10 +3507,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3326,10 +3551,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3370,10 +3595,10 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3414,10 +3639,10 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3458,10 +3683,10 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -3502,10 +3727,10 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3546,10 +3771,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -3590,10 +3815,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -3634,10 +3859,10 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -3678,10 +3903,10 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -3722,10 +3947,10 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -3766,10 +3991,10 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -3810,5 +4035,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finalize the class and hydrology ini file generation funcitons with examples and description
</commit_message>
<xml_diff>
--- a/MESHpyPreProcessing/meshparametersvalues2.xlsx
+++ b/MESHpyPreProcessing/meshparametersvalues2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\GitHub\Repos\MESH-Scripts-PyLib\MESHpyPreProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9464CC30-554B-46DB-AEAA-FDE1DDF58647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138AFD33-0DD8-4B4E-BD1E-97185B99BEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AC73AADA-9DAA-4E49-8D0A-BF563EF11B8B}"/>
   </bookViews>
@@ -2631,7 +2631,7 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>